<commit_message>
Worked on basis of selection, created template for generating training data, and implemented initial framework for parsing new data to create sparse matrix
</commit_message>
<xml_diff>
--- a/CDSData/CDS_SPARSE_2019_2020.xlsx
+++ b/CDSData/CDS_SPARSE_2019_2020.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\CDSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2904F4-C655-485A-9DD4-724A75CC56AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B93CC7-2EA9-4B5A-8CAD-65A8F616A267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cohort_Retentio" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,12 +26,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>retention-rate</t>
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>rigor of secondary school record</t>
+  </si>
+  <si>
+    <t>class rank</t>
+  </si>
+  <si>
+    <t>academic GPA</t>
+  </si>
+  <si>
+    <t>standardized test scores</t>
+  </si>
+  <si>
+    <t>application Essay</t>
+  </si>
+  <si>
+    <t>recommendation</t>
+  </si>
+  <si>
+    <t>interview</t>
+  </si>
+  <si>
+    <t>extracurricular activities</t>
+  </si>
+  <si>
+    <t>talent/ability</t>
+  </si>
+  <si>
+    <t>character/personal qualities</t>
+  </si>
+  <si>
+    <t>first generation</t>
+  </si>
+  <si>
+    <t>alumni/ae relation</t>
+  </si>
+  <si>
+    <t>geographical residence</t>
+  </si>
+  <si>
+    <t>state residency</t>
+  </si>
+  <si>
+    <t>religious affiliation/commitment</t>
+  </si>
+  <si>
+    <t>racial/ethnic status</t>
+  </si>
+  <si>
+    <t>volunteer work</t>
+  </si>
+  <si>
+    <t>work experience</t>
+  </si>
+  <si>
+    <t>level of applicant’s interest</t>
+  </si>
+  <si>
+    <t>Very Important</t>
+  </si>
+  <si>
+    <t>Considered</t>
   </si>
 </sst>
 </file>
@@ -350,7 +414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C948433-D7E6-473D-988C-F4FA96EE320C}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -378,4 +442,224 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5DC1794-7F0C-4BFD-A263-538507BB27B7}">
+  <dimension ref="A1:T5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:T5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>